<commit_message>
setactive and setinactive are both working, IP addresses updated
</commit_message>
<xml_diff>
--- a/db.xlsx
+++ b/db.xlsx
@@ -44,114 +44,6 @@
     <t>_id</t>
   </si>
   <si>
-    <t>00.00.000.00</t>
-  </si>
-  <si>
-    <t>11.11.111.11</t>
-  </si>
-  <si>
-    <t>22.22.222.22</t>
-  </si>
-  <si>
-    <t>33.33.333.33</t>
-  </si>
-  <si>
-    <t>44.44.444.44</t>
-  </si>
-  <si>
-    <t>55.55.555.55</t>
-  </si>
-  <si>
-    <t>66.66.666.66</t>
-  </si>
-  <si>
-    <t>77.77.777.77</t>
-  </si>
-  <si>
-    <t>88.88.888.88</t>
-  </si>
-  <si>
-    <t>99.99.999.99</t>
-  </si>
-  <si>
-    <t>00.00.111.11</t>
-  </si>
-  <si>
-    <t>00.00.222.22</t>
-  </si>
-  <si>
-    <t>00.00.333.33</t>
-  </si>
-  <si>
-    <t>00.00.444.44</t>
-  </si>
-  <si>
-    <t>00.00.555.55</t>
-  </si>
-  <si>
-    <t>00.00.666.66</t>
-  </si>
-  <si>
-    <t>00.00.777.77</t>
-  </si>
-  <si>
-    <t>00.00.888.88</t>
-  </si>
-  <si>
-    <t>00.00.999.99</t>
-  </si>
-  <si>
-    <t>11.11.000.00</t>
-  </si>
-  <si>
-    <t>22.22.000.00</t>
-  </si>
-  <si>
-    <t>33.33.000.00</t>
-  </si>
-  <si>
-    <t>44.44.000.00</t>
-  </si>
-  <si>
-    <t>55.55.000.00</t>
-  </si>
-  <si>
-    <t>66.66.000.00</t>
-  </si>
-  <si>
-    <t>77.77.000.00</t>
-  </si>
-  <si>
-    <t>88.88.000.00</t>
-  </si>
-  <si>
-    <t>99.99.000.00</t>
-  </si>
-  <si>
-    <t>12.34.567.89</t>
-  </si>
-  <si>
-    <t>98.76.543.21</t>
-  </si>
-  <si>
-    <t>24.68.101.21</t>
-  </si>
-  <si>
-    <t>13.57.911.13</t>
-  </si>
-  <si>
-    <t>12.12.121.12</t>
-  </si>
-  <si>
-    <t>23.23.232.23</t>
-  </si>
-  <si>
-    <t>34.34.343.34</t>
-  </si>
-  <si>
-    <t>45.45.454.45</t>
-  </si>
-  <si>
     <t>inactive</t>
   </si>
   <si>
@@ -261,6 +153,114 @@
   </si>
   <si>
     <t>HACdjSESraG9JAvXN</t>
+  </si>
+  <si>
+    <t>129.62.150.11</t>
+  </si>
+  <si>
+    <t>129.62.150.12</t>
+  </si>
+  <si>
+    <t>129.62.150.13</t>
+  </si>
+  <si>
+    <t>129.62.150.14</t>
+  </si>
+  <si>
+    <t>129.62.150.15</t>
+  </si>
+  <si>
+    <t>129.62.150.16</t>
+  </si>
+  <si>
+    <t>129.62.150.17</t>
+  </si>
+  <si>
+    <t>129.62.150.18</t>
+  </si>
+  <si>
+    <t>129.62.150.19</t>
+  </si>
+  <si>
+    <t>129.62.150.20</t>
+  </si>
+  <si>
+    <t>129.62.150.21</t>
+  </si>
+  <si>
+    <t>129.62.150.22</t>
+  </si>
+  <si>
+    <t>129.62.150.23</t>
+  </si>
+  <si>
+    <t>129.62.150.24</t>
+  </si>
+  <si>
+    <t>129.62.150.25</t>
+  </si>
+  <si>
+    <t>129.62.150.26</t>
+  </si>
+  <si>
+    <t>129.62.150.27</t>
+  </si>
+  <si>
+    <t>129.62.150.28</t>
+  </si>
+  <si>
+    <t>129.62.150.29</t>
+  </si>
+  <si>
+    <t>129.62.150.30</t>
+  </si>
+  <si>
+    <t>129.62.150.31</t>
+  </si>
+  <si>
+    <t>129.62.150.32</t>
+  </si>
+  <si>
+    <t>129.62.150.33</t>
+  </si>
+  <si>
+    <t>129.62.150.34</t>
+  </si>
+  <si>
+    <t>129.62.150.35</t>
+  </si>
+  <si>
+    <t>129.62.150.36</t>
+  </si>
+  <si>
+    <t>129.62.150.37</t>
+  </si>
+  <si>
+    <t>129.62.150.38</t>
+  </si>
+  <si>
+    <t>129.62.150.39</t>
+  </si>
+  <si>
+    <t>129.62.150.40</t>
+  </si>
+  <si>
+    <t>129.62.150.41</t>
+  </si>
+  <si>
+    <t>129.62.150.42</t>
+  </si>
+  <si>
+    <t>129.62.150.43</t>
+  </si>
+  <si>
+    <t>129.62.150.44</t>
+  </si>
+  <si>
+    <t>129.62.150.45</t>
+  </si>
+  <si>
+    <t>129.62.150.46</t>
   </si>
 </sst>
 </file>
@@ -617,13 +617,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="E38" sqref="E38"/>
+    <sheetView tabSelected="1" topLeftCell="A32" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.21875" customWidth="1"/>
+    <col min="1" max="1" width="12.88671875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="21.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -651,10 +651,10 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>67</v>
       </c>
       <c r="B3" t="s">
-        <v>42</v>
+        <v>6</v>
       </c>
       <c r="C3" s="1">
         <v>1</v>
@@ -663,15 +663,15 @@
         <v>1</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>43</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>68</v>
       </c>
       <c r="B4" t="s">
-        <v>42</v>
+        <v>6</v>
       </c>
       <c r="C4" s="1">
         <v>1</v>
@@ -680,15 +680,15 @@
         <v>2</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>44</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>69</v>
       </c>
       <c r="B5" t="s">
-        <v>42</v>
+        <v>6</v>
       </c>
       <c r="C5" s="1">
         <v>1</v>
@@ -697,15 +697,15 @@
         <v>3</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>45</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>70</v>
       </c>
       <c r="B6" t="s">
-        <v>42</v>
+        <v>6</v>
       </c>
       <c r="C6" s="1">
         <v>1</v>
@@ -714,15 +714,15 @@
         <v>4</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>46</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>71</v>
       </c>
       <c r="B7" t="s">
-        <v>42</v>
+        <v>6</v>
       </c>
       <c r="C7" s="1">
         <v>1</v>
@@ -731,15 +731,15 @@
         <v>5</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>47</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>11</v>
+        <v>72</v>
       </c>
       <c r="B8" t="s">
-        <v>42</v>
+        <v>6</v>
       </c>
       <c r="C8" s="1">
         <v>1</v>
@@ -748,15 +748,15 @@
         <v>6</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>48</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>12</v>
+        <v>73</v>
       </c>
       <c r="B9" t="s">
-        <v>42</v>
+        <v>6</v>
       </c>
       <c r="C9" s="1">
         <v>1</v>
@@ -765,15 +765,15 @@
         <v>7</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>49</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>13</v>
+        <v>74</v>
       </c>
       <c r="B10" t="s">
-        <v>42</v>
+        <v>6</v>
       </c>
       <c r="C10" s="1">
         <v>1</v>
@@ -782,15 +782,15 @@
         <v>8</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>50</v>
+        <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>14</v>
+        <v>75</v>
       </c>
       <c r="B11" t="s">
-        <v>42</v>
+        <v>6</v>
       </c>
       <c r="C11" s="1">
         <v>1</v>
@@ -799,15 +799,15 @@
         <v>9</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>51</v>
+        <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>15</v>
+        <v>76</v>
       </c>
       <c r="B12" t="s">
-        <v>42</v>
+        <v>6</v>
       </c>
       <c r="C12" s="1">
         <v>1</v>
@@ -816,15 +816,15 @@
         <v>10</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>52</v>
+        <v>16</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>16</v>
+        <v>77</v>
       </c>
       <c r="B13" t="s">
-        <v>42</v>
+        <v>6</v>
       </c>
       <c r="C13" s="1">
         <v>1</v>
@@ -833,15 +833,15 @@
         <v>11</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>53</v>
+        <v>17</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>17</v>
+        <v>78</v>
       </c>
       <c r="B14" t="s">
-        <v>42</v>
+        <v>6</v>
       </c>
       <c r="C14" s="1">
         <v>1</v>
@@ -850,15 +850,15 @@
         <v>12</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>54</v>
+        <v>18</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>18</v>
+        <v>55</v>
       </c>
       <c r="B15" t="s">
-        <v>42</v>
+        <v>6</v>
       </c>
       <c r="C15" s="1">
         <v>2</v>
@@ -867,15 +867,15 @@
         <v>13</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>55</v>
+        <v>19</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>19</v>
+        <v>56</v>
       </c>
       <c r="B16" t="s">
-        <v>42</v>
+        <v>6</v>
       </c>
       <c r="C16" s="1">
         <v>2</v>
@@ -884,15 +884,15 @@
         <v>14</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>56</v>
+        <v>20</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>20</v>
+        <v>57</v>
       </c>
       <c r="B17" t="s">
-        <v>42</v>
+        <v>6</v>
       </c>
       <c r="C17" s="1">
         <v>2</v>
@@ -901,15 +901,15 @@
         <v>15</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>57</v>
+        <v>21</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>21</v>
+        <v>58</v>
       </c>
       <c r="B18" t="s">
-        <v>42</v>
+        <v>6</v>
       </c>
       <c r="C18" s="1">
         <v>2</v>
@@ -918,15 +918,15 @@
         <v>16</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>58</v>
+        <v>22</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>22</v>
+        <v>59</v>
       </c>
       <c r="B19" t="s">
-        <v>42</v>
+        <v>6</v>
       </c>
       <c r="C19" s="1">
         <v>2</v>
@@ -935,15 +935,15 @@
         <v>17</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>59</v>
+        <v>23</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>23</v>
+        <v>60</v>
       </c>
       <c r="B20" t="s">
-        <v>42</v>
+        <v>6</v>
       </c>
       <c r="C20" s="1">
         <v>2</v>
@@ -952,15 +952,15 @@
         <v>18</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>60</v>
+        <v>24</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>24</v>
+        <v>61</v>
       </c>
       <c r="B21" t="s">
-        <v>42</v>
+        <v>6</v>
       </c>
       <c r="C21" s="1">
         <v>2</v>
@@ -969,15 +969,15 @@
         <v>19</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>61</v>
+        <v>25</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>25</v>
+        <v>62</v>
       </c>
       <c r="B22" t="s">
-        <v>42</v>
+        <v>6</v>
       </c>
       <c r="C22" s="1">
         <v>2</v>
@@ -986,15 +986,15 @@
         <v>20</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>62</v>
+        <v>26</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>26</v>
+        <v>63</v>
       </c>
       <c r="B23" t="s">
-        <v>42</v>
+        <v>6</v>
       </c>
       <c r="C23" s="1">
         <v>2</v>
@@ -1003,15 +1003,15 @@
         <v>21</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>63</v>
+        <v>27</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>27</v>
+        <v>64</v>
       </c>
       <c r="B24" t="s">
-        <v>42</v>
+        <v>6</v>
       </c>
       <c r="C24" s="1">
         <v>2</v>
@@ -1020,15 +1020,15 @@
         <v>22</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>64</v>
+        <v>28</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>28</v>
+        <v>65</v>
       </c>
       <c r="B25" t="s">
-        <v>42</v>
+        <v>6</v>
       </c>
       <c r="C25" s="1">
         <v>2</v>
@@ -1037,15 +1037,15 @@
         <v>23</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>65</v>
+        <v>29</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>29</v>
+        <v>66</v>
       </c>
       <c r="B26" t="s">
-        <v>42</v>
+        <v>6</v>
       </c>
       <c r="C26" s="1">
         <v>2</v>
@@ -1054,15 +1054,15 @@
         <v>24</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>66</v>
+        <v>30</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="B27" t="s">
-        <v>42</v>
+        <v>6</v>
       </c>
       <c r="C27" s="1">
         <v>3</v>
@@ -1071,15 +1071,15 @@
         <v>25</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>67</v>
+        <v>31</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>31</v>
+        <v>44</v>
       </c>
       <c r="B28" t="s">
-        <v>42</v>
+        <v>6</v>
       </c>
       <c r="C28" s="1">
         <v>3</v>
@@ -1088,15 +1088,15 @@
         <v>26</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>68</v>
+        <v>32</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>32</v>
+        <v>45</v>
       </c>
       <c r="B29" t="s">
-        <v>42</v>
+        <v>6</v>
       </c>
       <c r="C29" s="1">
         <v>3</v>
@@ -1105,15 +1105,15 @@
         <v>27</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>69</v>
+        <v>33</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>33</v>
+        <v>46</v>
       </c>
       <c r="B30" t="s">
-        <v>42</v>
+        <v>6</v>
       </c>
       <c r="C30" s="1">
         <v>3</v>
@@ -1122,15 +1122,15 @@
         <v>28</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>70</v>
+        <v>34</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>34</v>
+        <v>47</v>
       </c>
       <c r="B31" t="s">
-        <v>42</v>
+        <v>6</v>
       </c>
       <c r="C31" s="1">
         <v>3</v>
@@ -1139,15 +1139,15 @@
         <v>29</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>71</v>
+        <v>35</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>35</v>
+        <v>48</v>
       </c>
       <c r="B32" t="s">
-        <v>42</v>
+        <v>6</v>
       </c>
       <c r="C32" s="1">
         <v>3</v>
@@ -1156,15 +1156,15 @@
         <v>30</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>72</v>
+        <v>36</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>36</v>
+        <v>49</v>
       </c>
       <c r="B33" t="s">
-        <v>42</v>
+        <v>6</v>
       </c>
       <c r="C33" s="1">
         <v>3</v>
@@ -1173,15 +1173,15 @@
         <v>31</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>73</v>
+        <v>37</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>37</v>
+        <v>50</v>
       </c>
       <c r="B34" t="s">
-        <v>42</v>
+        <v>6</v>
       </c>
       <c r="C34" s="1">
         <v>3</v>
@@ -1190,15 +1190,15 @@
         <v>32</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>74</v>
+        <v>38</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>38</v>
+        <v>51</v>
       </c>
       <c r="B35" t="s">
-        <v>42</v>
+        <v>6</v>
       </c>
       <c r="C35" s="1">
         <v>3</v>
@@ -1207,15 +1207,15 @@
         <v>33</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>75</v>
+        <v>39</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>39</v>
+        <v>52</v>
       </c>
       <c r="B36" t="s">
-        <v>42</v>
+        <v>6</v>
       </c>
       <c r="C36" s="1">
         <v>3</v>
@@ -1224,15 +1224,15 @@
         <v>34</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>76</v>
+        <v>40</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>40</v>
+        <v>53</v>
       </c>
       <c r="B37" t="s">
-        <v>42</v>
+        <v>6</v>
       </c>
       <c r="C37" s="1">
         <v>3</v>
@@ -1241,15 +1241,15 @@
         <v>35</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>77</v>
+        <v>41</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>41</v>
+        <v>54</v>
       </c>
       <c r="B38" t="s">
-        <v>42</v>
+        <v>6</v>
       </c>
       <c r="C38" s="1">
         <v>3</v>
@@ -1258,7 +1258,7 @@
         <v>36</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>78</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>